<commit_message>
Minor updates on main site template for xls reports
</commit_message>
<xml_diff>
--- a/storage/templates/reports.xlsx
+++ b/storage/templates/reports.xlsx
@@ -19,12 +19,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">The Ultimate Care Rentals Management System</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -45,6 +53,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -61,12 +76,68 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+  <borders count="9">
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -95,12 +166,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,15 +296,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1158840</xdr:colOff>
+      <xdr:colOff>978840</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>100800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2338560</xdr:colOff>
+      <xdr:colOff>2158200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -202,8 +317,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5245560" y="100800"/>
-          <a:ext cx="2437560" cy="380520"/>
+          <a:off x="5065560" y="100800"/>
+          <a:ext cx="2437200" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -223,13 +338,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.19"/>
@@ -237,19 +352,33 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="AMJ1" s="3"/>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="AMJ2" s="6"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="AMJ3" s="6"/>
+    </row>
+    <row r="4" s="9" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="D4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="AMJ4" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="1:4"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>